<commit_message>
Start tracking .xls & .xlsx in git lfs
</commit_message>
<xml_diff>
--- a/+DataKit/ressources/validMethods.xlsx
+++ b/+DataKit/ressources/validMethods.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/David/Dropbox/David/Syncing/MATLAB/toolboxes/+DataKit/ressources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/David/Dropbox/David/Syncing/MATLAB/toolboxes/Dingi/+DataKit/ressources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E22122-0301-B34E-B699-697B61E8D7F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E9ED73-FD40-974A-9A72-7FBAF14A27B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23400" yWindow="12860" windowWidth="26840" windowHeight="15940" xr2:uid="{F601EB49-FD18-B340-B36D-06ABFB19DC48}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>MethodId</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>ion chromatography</t>
+  </si>
+  <si>
+    <t>ICP-MS</t>
+  </si>
+  <si>
+    <t>inductively-coupled-plasma mass-spectrometry</t>
+  </si>
+  <si>
+    <t>DIC analyzer</t>
   </si>
 </sst>
 </file>
@@ -414,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA5AF89-7266-3C43-B728-2819F851858D}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -423,7 +432,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="109.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -478,6 +487,25 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement analysis changes into GearKit
</commit_message>
<xml_diff>
--- a/+DataKit/ressources/validMethods.xlsx
+++ b/+DataKit/ressources/validMethods.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/David/Dropbox/David/Syncing/MATLAB/toolboxes/+DataKit/ressources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/David/Dropbox/David/Syncing/MATLAB/toolboxes/Dingi/+DataKit/ressources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E22122-0301-B34E-B699-697B61E8D7F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823321D4-2F2D-764D-A13D-F7AF627F249D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23400" yWindow="12860" windowWidth="26840" windowHeight="15940" xr2:uid="{F601EB49-FD18-B340-B36D-06ABFB19DC48}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>MethodId</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>ion chromatography</t>
+  </si>
+  <si>
+    <t>ICP-MS</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA5AF89-7266-3C43-B728-2819F851858D}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,6 +481,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>